<commit_message>
[master] finished  update php tutorial 5
</commit_message>
<xml_diff>
--- a/review/review_points_HeinHtetSan.xlsx
+++ b/review/review_points_HeinHtetSan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BiB Training\PHP installation\apache\Apache24\htdocs\PHP-Training\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -193,7 +193,36 @@
 index.php</t>
   </si>
   <si>
-    <t>change 4 sapce</t>
+    <t>Tutorial_03
+index.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Use an indent of 4 spaces for *.php
+2) When enter future date,instead of showing your age is 0,
+   use condition to show message for Invalid DOB.
+3) Use proper name </t>
+  </si>
+  <si>
+    <t>change 4 space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) change 4 space
+2)  show message  DOB.
+3) Use proper name </t>
+  </si>
+  <si>
+    <t>Tutorial_04
+index.php</t>
+  </si>
+  <si>
+    <t>1) change 4 space
+2)  set connection Login
+3) connectin not accept null data</t>
+  </si>
+  <si>
+    <t>1) Use an indent of 4 spaces for *.php
+2) Please set default username and password to show Invalid Login
+3) Need form validation (not form accepting null data)</t>
   </si>
 </sst>
 </file>
@@ -1383,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:U4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1486,7 +1515,7 @@
         <v>27</v>
       </c>
       <c r="P2" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="29"/>
       <c r="R2" s="29"/>
@@ -1494,7 +1523,7 @@
       <c r="T2" s="29"/>
       <c r="U2" s="30"/>
       <c r="V2" s="21">
-        <v>44546.083333333336</v>
+        <v>44546.583333333336</v>
       </c>
       <c r="W2" s="18" t="s">
         <v>28</v>
@@ -1534,7 +1563,7 @@
         <v>27</v>
       </c>
       <c r="P3" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -1542,7 +1571,7 @@
       <c r="T3" s="29"/>
       <c r="U3" s="30"/>
       <c r="V3" s="21">
-        <v>44546.083333333336</v>
+        <v>44546.583333333336</v>
       </c>
       <c r="W3" s="18" t="s">
         <v>28</v>
@@ -1555,24 +1584,36 @@
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="25"/>
+      <c r="F4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="27"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
+      <c r="O4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="21">
+        <v>44547.833333333336</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="X4" s="18"/>
     </row>
     <row r="5" spans="1:24" ht="135" customHeight="1">
@@ -1581,24 +1622,36 @@
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="41"/>
+      <c r="F5" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
-      <c r="I5" s="25"/>
+      <c r="I5" s="25" t="s">
+        <v>39</v>
+      </c>
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="27"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
+      <c r="O5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="21">
+        <v>44547.833333333336</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="X5" s="18"/>
     </row>
     <row r="6" spans="1:24" ht="135" customHeight="1">

</xml_diff>

<commit_message>
[master] finished update  review
</commit_message>
<xml_diff>
--- a/review/review_points_HeinHtetSan.xlsx
+++ b/review/review_points_HeinHtetSan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -489,6 +489,57 @@
     <xf numFmtId="22" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -497,57 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +586,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:N5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1448,30 +1448,30 @@
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="24"/>
       <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="27"/>
       <c r="V1" s="17" t="s">
         <v>16</v>
       </c>
@@ -1498,30 +1498,30 @@
       <c r="E2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="25" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="40"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="34"/>
       <c r="O2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="21">
         <v>44546.583333333336</v>
       </c>
@@ -1546,30 +1546,30 @@
       <c r="E3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="25" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="34"/>
       <c r="O3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="37"/>
       <c r="V3" s="21">
         <v>44546.583333333336</v>
       </c>
@@ -1579,35 +1579,45 @@
       <c r="X3" s="18"/>
     </row>
     <row r="4" spans="1:24" ht="135" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="25" t="s">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20">
+        <v>44547</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="25" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="27"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="27"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="30"/>
       <c r="V4" s="21">
         <v>44547.833333333336</v>
       </c>
@@ -1617,35 +1627,45 @@
       <c r="X4" s="18"/>
     </row>
     <row r="5" spans="1:24" ht="135" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="41" t="s">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20">
+        <v>44547</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="25" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="27"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="27"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
       <c r="V5" s="21">
         <v>44547.833333333336</v>
       </c>
@@ -1660,22 +1680,22 @@
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="24"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="41"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="30"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="37"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
       <c r="X6" s="18"/>
@@ -1686,28 +1706,33 @@
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="40"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="F1:H1"/>
@@ -1724,11 +1749,6 @@
     <mergeCell ref="I4:N4"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="P5:U5"/>
-    <mergeCell ref="P6:U6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>